<commit_message>
situacioni done dashnia done
</commit_message>
<xml_diff>
--- a/1-Situacioni/regjistri/18-Koordinatat-e-ndërtesës1819-1-Varosh-Milaimi-leg.xlsx
+++ b/1-Situacioni/regjistri/18-Koordinatat-e-ndërtesës1819-1-Varosh-Milaimi-leg.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Ferizaj\Greme\Ingjinjerike\173-4-Greme-Ademi\1-Situacioni\regjistri\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ferizaj\Varosh\ing\1819-1-Varosh-Milaimi-leg\1-Situacioni\regjistri\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F2A2A1-FE3F-46E9-ADF7-0B7B66CC031E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$K$41</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
   <si>
     <t>Nr</t>
   </si>
@@ -80,9 +80,6 @@
     <t>STREHA</t>
   </si>
   <si>
-    <t>KULMI</t>
-  </si>
-  <si>
     <t>PERDHESA</t>
   </si>
   <si>
@@ -98,31 +95,46 @@
     <t>PERDHESA-TERAS</t>
   </si>
   <si>
-    <t>BUNARI</t>
+    <t>ci_a_p1</t>
   </si>
   <si>
-    <t>FS1</t>
+    <t>ci_a_p2</t>
   </si>
   <si>
-    <t>FS2</t>
+    <t>ci_a_p3</t>
   </si>
   <si>
-    <t>P1</t>
+    <t>ci_va_fs1</t>
   </si>
   <si>
-    <t>P2</t>
+    <t>kulmi</t>
   </si>
   <si>
-    <t>P5</t>
+    <t>kyqje_uj</t>
   </si>
   <si>
-    <t>KYQJE-ELEKTRIKE</t>
+    <t>perdhese</t>
+  </si>
+  <si>
+    <t>perdhese-terasa</t>
+  </si>
+  <si>
+    <t>perdhese-terase</t>
+  </si>
+  <si>
+    <t>pusetFeekkal</t>
+  </si>
+  <si>
+    <t>shtylElektrike</t>
+  </si>
+  <si>
+    <t>streha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -479,7 +491,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -795,21 +807,6 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -937,22 +934,22 @@
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -978,7 +975,7 @@
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -986,7 +983,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1004,24 +1001,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1031,19 +1016,16 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1056,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1071,7 +1053,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1380,7 +1362,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Greme</a:t>
+            <a:t>Varosh</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1483,16 +1465,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>00173-4</a:t>
+            <a:t>01819-1</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="1" smtClean="0">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1400" b="1">
@@ -1879,11 +1853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,112 +1873,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
     </row>
     <row r="2" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
-      <c r="K4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
     </row>
     <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="31"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="34"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="36"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
@@ -2032,16 +2006,16 @@
     </row>
     <row r="15" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C15" s="9">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D15" s="10">
-        <v>7512915.9336999999</v>
+        <v>7515264.8969999999</v>
       </c>
       <c r="E15" s="10">
-        <v>4688194.9045000002</v>
+        <v>4688743.5379999997</v>
       </c>
       <c r="F15" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G15" s="7">
         <v>40</v>
@@ -2055,16 +2029,16 @@
     </row>
     <row r="16" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C16" s="9">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="D16" s="10">
-        <v>7512912.4574999996</v>
+        <v>7515261.9819</v>
       </c>
       <c r="E16" s="10">
-        <v>4688193.57</v>
+        <v>4688748.426</v>
       </c>
       <c r="F16" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G16" s="7">
         <v>40</v>
@@ -2078,16 +2052,16 @@
     </row>
     <row r="17" spans="1:11" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C17" s="9">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="D17" s="10">
-        <v>7512912.7120000003</v>
+        <v>7515258.2007999998</v>
       </c>
       <c r="E17" s="10">
-        <v>4688192.9069999997</v>
+        <v>4688732.3382999999</v>
       </c>
       <c r="F17" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G17" s="7">
         <v>40</v>
@@ -2103,16 +2077,16 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="9">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="D18" s="10">
-        <v>7512908.3671000004</v>
+        <v>7515255.392</v>
       </c>
       <c r="E18" s="10">
-        <v>4688191.2390000001</v>
+        <v>4688748.3090000004</v>
       </c>
       <c r="F18" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G18" s="7">
         <v>40</v>
@@ -2130,16 +2104,16 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="9">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="D19" s="10">
-        <v>7512905.0319999997</v>
+        <v>7515250.4359999998</v>
       </c>
       <c r="E19" s="10">
-        <v>4688199.3990000002</v>
+        <v>4688745.358</v>
       </c>
       <c r="F19" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G19" s="7">
         <v>40</v>
@@ -2157,16 +2131,16 @@
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="9">
-        <v>167</v>
+        <v>63</v>
       </c>
       <c r="D20" s="10">
-        <v>7512912.8032999998</v>
+        <v>7515257.0695000002</v>
       </c>
       <c r="E20" s="10">
-        <v>4688202.5635000002</v>
+        <v>4688745.4962999998</v>
       </c>
       <c r="F20" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G20" s="7">
         <v>40</v>
@@ -2184,16 +2158,16 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="9">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="D21" s="10">
-        <v>7512916.9979999997</v>
+        <v>7515265.5976</v>
       </c>
       <c r="E21" s="10">
-        <v>4688192.1320000002</v>
+        <v>4688738.6950000003</v>
       </c>
       <c r="F21" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G21" s="7">
         <v>40</v>
@@ -2211,16 +2185,16 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="9">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="D22" s="10">
-        <v>7512911.5231999997</v>
+        <v>7515261.3786000004</v>
       </c>
       <c r="E22" s="10">
-        <v>4688192.4506000001</v>
+        <v>4688734.2335000001</v>
       </c>
       <c r="F22" s="10">
-        <v>601.94100000000003</v>
+        <v>588.41700000000003</v>
       </c>
       <c r="G22" s="7">
         <v>40</v>
@@ -2234,28 +2208,28 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="11">
-        <v>13</v>
-      </c>
-      <c r="D23" s="12">
-        <v>7512912.3669999996</v>
-      </c>
-      <c r="E23" s="12">
-        <v>4688190.3370000003</v>
-      </c>
-      <c r="F23" s="12">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="G23" s="13">
+      <c r="C23" s="9">
+        <v>83</v>
+      </c>
+      <c r="D23" s="10">
+        <v>7515263.2832000004</v>
+      </c>
+      <c r="E23" s="10">
+        <v>4688742.5756000001</v>
+      </c>
+      <c r="F23" s="10">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="G23" s="7">
         <v>40</v>
       </c>
-      <c r="H23" s="13" t="s">
+      <c r="H23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J23" s="4"/>
@@ -2264,143 +2238,157 @@
     <row r="24" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="26"/>
+      <c r="C24" s="9">
+        <v>85</v>
+      </c>
+      <c r="D24" s="10">
+        <v>7515260.5228000004</v>
+      </c>
+      <c r="E24" s="10">
+        <v>4688735.6684999997</v>
+      </c>
+      <c r="F24" s="10">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="G24" s="7">
+        <v>40</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="26"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="22"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="26"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="22"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="26"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="22"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="26"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="26"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="22"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="26"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="22"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
     </row>
     <row r="31" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="26"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="22"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="26"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="22"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
     </row>
     <row r="33" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="26"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="22"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
     </row>
     <row r="34" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="26"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="22"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
@@ -2456,34 +2444,34 @@
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="46"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="42" t="s">
+      <c r="E40" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="39"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I40" s="43"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="54"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="47"/>
     </row>
     <row r="41" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="48" t="s">
+      <c r="A41" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="51">
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="44">
         <v>140</v>
       </c>
-      <c r="F41" s="51"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="44"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="55"/>
-      <c r="K41" s="56"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="49"/>
     </row>
     <row r="42" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="K42" s="4"/>
@@ -2512,11 +2500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E7:O30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="E7:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:H25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,679 +2520,747 @@
   <sheetData>
     <row r="7" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="20" t="s">
+      <c r="I8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="L8" s="21" t="s">
+      <c r="L8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="M8" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="N8" s="21" t="s">
+      <c r="N8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E9" s="17">
-        <v>8</v>
-      </c>
-      <c r="F9" s="16">
-        <v>7512917.0159999998</v>
-      </c>
-      <c r="G9" s="16">
-        <v>4688188.8219999997</v>
-      </c>
-      <c r="H9" s="16">
-        <v>601.84799999999996</v>
-      </c>
-      <c r="I9" s="19" t="s">
+      <c r="E9" s="13">
+        <v>79</v>
+      </c>
+      <c r="F9" s="12">
+        <v>7515278.8360000001</v>
+      </c>
+      <c r="G9" s="12">
+        <v>4688777.6189999999</v>
+      </c>
+      <c r="H9" s="12">
+        <v>588.03700000000003</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="13">
+        <v>125</v>
+      </c>
+      <c r="L9" s="12">
+        <v>7513330.0590000004</v>
+      </c>
+      <c r="M9" s="12">
+        <v>4690846.6090000002</v>
+      </c>
+      <c r="N9" s="12">
+        <v>605.072</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="18">
+        <v>80</v>
+      </c>
+      <c r="F10" s="14">
+        <v>7515281.8449999997</v>
+      </c>
+      <c r="G10" s="14">
+        <v>4688734.4840000002</v>
+      </c>
+      <c r="H10" s="14">
+        <v>588.01</v>
+      </c>
+      <c r="I10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="17">
-        <v>125</v>
-      </c>
-      <c r="L9" s="16">
-        <v>7513330.0590000004</v>
-      </c>
-      <c r="M9" s="16">
-        <v>4690846.6090000002</v>
-      </c>
-      <c r="N9" s="16">
+      <c r="K10" s="18">
+        <v>126</v>
+      </c>
+      <c r="L10" s="14">
+        <v>7513338.2350000003</v>
+      </c>
+      <c r="M10" s="14">
+        <v>4690858.04</v>
+      </c>
+      <c r="N10" s="14">
         <v>605.072</v>
       </c>
-      <c r="O9" s="19" t="s">
+      <c r="O10" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="18">
+        <v>81</v>
+      </c>
+      <c r="F11" s="14">
+        <v>7515239.7510000002</v>
+      </c>
+      <c r="G11" s="14">
+        <v>4688740.3499999996</v>
+      </c>
+      <c r="H11" s="14">
+        <v>587.71600000000001</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="18">
+        <v>14</v>
+      </c>
+      <c r="L11" s="14">
+        <v>7513349.2649999997</v>
+      </c>
+      <c r="M11" s="14">
+        <v>4690850.0329999998</v>
+      </c>
+      <c r="N11" s="14">
+        <v>605.072</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="18">
+        <v>82</v>
+      </c>
+      <c r="F12" s="14">
+        <v>7515266.1509999996</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4688757.7439999999</v>
+      </c>
+      <c r="H12" s="14">
+        <v>589.54999999999995</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="18">
+        <v>15</v>
+      </c>
+      <c r="L12" s="14">
+        <v>7513344.9910000004</v>
+      </c>
+      <c r="M12" s="14">
+        <v>4690844.074</v>
+      </c>
+      <c r="N12" s="14">
+        <v>605.072</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="18">
+        <v>70</v>
+      </c>
+      <c r="F13" s="14">
+        <v>7515256.9780000001</v>
+      </c>
+      <c r="G13" s="14">
+        <v>4688745.5810000002</v>
+      </c>
+      <c r="H13" s="14">
+        <v>595.24400000000003</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="18">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E10" s="22">
-        <v>159</v>
-      </c>
-      <c r="F10" s="18">
-        <v>7512898.091</v>
-      </c>
-      <c r="G10" s="18">
-        <v>4688178.9879999999</v>
-      </c>
-      <c r="H10" s="18">
-        <v>602.24300000000005</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="22">
-        <v>126</v>
-      </c>
-      <c r="L10" s="18">
-        <v>7513338.2350000003</v>
-      </c>
-      <c r="M10" s="18">
-        <v>4690858.04</v>
-      </c>
-      <c r="N10" s="18">
-        <v>605.072</v>
-      </c>
-      <c r="O10" s="15" t="s">
+      <c r="L13" s="14">
+        <v>7513351.2439999999</v>
+      </c>
+      <c r="M13" s="14">
+        <v>4690805.4189999998</v>
+      </c>
+      <c r="N13" s="14">
+        <v>604.52499999999998</v>
+      </c>
+      <c r="O13" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E11" s="22">
-        <v>160</v>
-      </c>
-      <c r="F11" s="18">
-        <v>7512898.0889999997</v>
-      </c>
-      <c r="G11" s="18">
-        <v>4688178.9890000001</v>
-      </c>
-      <c r="H11" s="18">
-        <v>602.24199999999996</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="22">
+    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="18">
+        <v>54</v>
+      </c>
+      <c r="F14" s="14">
+        <v>7515262.8229999999</v>
+      </c>
+      <c r="G14" s="14">
+        <v>4688748.216</v>
+      </c>
+      <c r="H14" s="14">
+        <v>587.93499999999995</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="18">
+        <v>18</v>
+      </c>
+      <c r="L14" s="14">
+        <v>7513361.0970000001</v>
+      </c>
+      <c r="M14" s="14">
+        <v>4690822.32</v>
+      </c>
+      <c r="N14" s="14">
+        <v>604.64200000000005</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="18">
+        <v>56</v>
+      </c>
+      <c r="F15" s="14">
+        <v>7515264.8969999999</v>
+      </c>
+      <c r="G15" s="14">
+        <v>4688743.5379999997</v>
+      </c>
+      <c r="H15" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15" s="18">
+        <v>19</v>
+      </c>
+      <c r="L15" s="14">
+        <v>7513378.5779999997</v>
+      </c>
+      <c r="M15" s="14">
+        <v>4690849.2640000004</v>
+      </c>
+      <c r="N15" s="14">
+        <v>604.70899999999995</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E16" s="18">
+        <v>59</v>
+      </c>
+      <c r="F16" s="14">
+        <v>7515261.9819</v>
+      </c>
+      <c r="G16" s="14">
+        <v>4688748.426</v>
+      </c>
+      <c r="H16" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" s="18">
+        <v>123</v>
+      </c>
+      <c r="L16" s="14">
+        <v>7513330.2640000004</v>
+      </c>
+      <c r="M16" s="14">
+        <v>4690842.0870000003</v>
+      </c>
+      <c r="N16" s="14">
+        <v>605.05399999999997</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E17" s="18">
+        <v>60</v>
+      </c>
+      <c r="F17" s="14">
+        <v>7515258.2007999998</v>
+      </c>
+      <c r="G17" s="14">
+        <v>4688732.3382999999</v>
+      </c>
+      <c r="H17" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="18">
+        <v>17</v>
+      </c>
+      <c r="L17" s="14">
+        <v>7513358.5389999999</v>
+      </c>
+      <c r="M17" s="14">
+        <v>4690822.3590000002</v>
+      </c>
+      <c r="N17" s="14">
+        <v>604.60199999999998</v>
+      </c>
+      <c r="O17" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E18" s="18">
+        <v>61</v>
+      </c>
+      <c r="F18" s="14">
+        <v>7515255.392</v>
+      </c>
+      <c r="G18" s="14">
+        <v>4688748.3090000004</v>
+      </c>
+      <c r="H18" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="18">
+        <v>20</v>
+      </c>
+      <c r="L18" s="14">
+        <v>7513386.9630000005</v>
+      </c>
+      <c r="M18" s="14">
+        <v>4690862.8320000004</v>
+      </c>
+      <c r="N18" s="14">
+        <v>604.92899999999997</v>
+      </c>
+      <c r="O18" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E19" s="18">
+        <v>62</v>
+      </c>
+      <c r="F19" s="14">
+        <v>7515250.4359999998</v>
+      </c>
+      <c r="G19" s="14">
+        <v>4688745.358</v>
+      </c>
+      <c r="H19" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="18">
+        <v>69</v>
+      </c>
+      <c r="L19" s="14">
+        <v>7513337.3779999996</v>
+      </c>
+      <c r="M19" s="14">
+        <v>4690836.5530000003</v>
+      </c>
+      <c r="N19" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="18">
-        <v>7513349.2649999997</v>
-      </c>
-      <c r="M11" s="18">
-        <v>4690850.0329999998</v>
-      </c>
-      <c r="N11" s="18">
-        <v>605.072</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E12" s="22">
-        <v>24</v>
-      </c>
-      <c r="F12" s="18">
-        <v>7512911.3329999996</v>
-      </c>
-      <c r="G12" s="18">
-        <v>4688194.7120000003</v>
-      </c>
-      <c r="H12" s="18">
-        <v>611.86400000000003</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="22">
-        <v>15</v>
-      </c>
-      <c r="L12" s="18">
-        <v>7513344.9910000004</v>
-      </c>
-      <c r="M12" s="18">
-        <v>4690844.074</v>
-      </c>
-      <c r="N12" s="18">
-        <v>605.072</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E13" s="22">
-        <v>17</v>
-      </c>
-      <c r="F13" s="18">
-        <v>7512915.8265000004</v>
-      </c>
-      <c r="G13" s="18">
-        <v>4688195.8137999997</v>
-      </c>
-      <c r="H13" s="18">
-        <v>601.69299999999998</v>
-      </c>
-      <c r="I13" s="15" t="s">
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E20" s="18">
+        <v>63</v>
+      </c>
+      <c r="F20" s="14">
+        <v>7515257.0695000002</v>
+      </c>
+      <c r="G20" s="14">
+        <v>4688745.4962999998</v>
+      </c>
+      <c r="H20" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="18">
+        <v>70</v>
+      </c>
+      <c r="L20" s="14">
+        <v>7513343.1220000004</v>
+      </c>
+      <c r="M20" s="14">
+        <v>4690844.5829999996</v>
+      </c>
+      <c r="N20" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O20" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E21" s="18">
+        <v>64</v>
+      </c>
+      <c r="F21" s="14">
+        <v>7515265.5976</v>
+      </c>
+      <c r="G21" s="14">
+        <v>4688738.6950000003</v>
+      </c>
+      <c r="H21" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="18">
+        <v>71</v>
+      </c>
+      <c r="L21" s="14">
+        <v>7513345.1220000004</v>
+      </c>
+      <c r="M21" s="14">
+        <v>4690843.176</v>
+      </c>
+      <c r="N21" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O21" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E22" s="18">
+        <v>74</v>
+      </c>
+      <c r="F22" s="14">
+        <v>7515261.3786000004</v>
+      </c>
+      <c r="G22" s="14">
+        <v>4688734.2335000001</v>
+      </c>
+      <c r="H22" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="18">
+        <v>72</v>
+      </c>
+      <c r="L22" s="14">
+        <v>7513350.1349999998</v>
+      </c>
+      <c r="M22" s="14">
+        <v>4690850.1849999996</v>
+      </c>
+      <c r="N22" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" s="18">
+        <v>83</v>
+      </c>
+      <c r="F23" s="14">
+        <v>7515263.2832000004</v>
+      </c>
+      <c r="G23" s="14">
+        <v>4688742.5756000001</v>
+      </c>
+      <c r="H23" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="18">
+        <v>130</v>
+      </c>
+      <c r="L23" s="14">
+        <v>7513331.6660000002</v>
+      </c>
+      <c r="M23" s="14">
+        <v>4690840.7719999999</v>
+      </c>
+      <c r="N23" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O23" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E24" s="18">
+        <v>85</v>
+      </c>
+      <c r="F24" s="14">
+        <v>7515260.5228000004</v>
+      </c>
+      <c r="G24" s="14">
+        <v>4688735.6684999997</v>
+      </c>
+      <c r="H24" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="18">
+        <v>131</v>
+      </c>
+      <c r="L24" s="14">
+        <v>7513333.6530999998</v>
+      </c>
+      <c r="M24" s="14">
+        <v>4690843.4441</v>
+      </c>
+      <c r="N24" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O24" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" s="18">
+        <v>57</v>
+      </c>
+      <c r="F25" s="14">
+        <v>7515266.0319999997</v>
+      </c>
+      <c r="G25" s="14">
+        <v>4688744.8449999997</v>
+      </c>
+      <c r="H25" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="22">
-        <v>16</v>
-      </c>
-      <c r="L13" s="18">
-        <v>7513351.2439999999</v>
-      </c>
-      <c r="M13" s="18">
-        <v>4690805.4189999998</v>
-      </c>
-      <c r="N13" s="18">
-        <v>604.52499999999998</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E14" s="22">
-        <v>151</v>
-      </c>
-      <c r="F14" s="18">
-        <v>7512909.4939999999</v>
-      </c>
-      <c r="G14" s="18">
-        <v>4688188.5990000004</v>
-      </c>
-      <c r="H14" s="18">
-        <v>601.99900000000002</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K14" s="22">
-        <v>18</v>
-      </c>
-      <c r="L14" s="18">
-        <v>7513361.0970000001</v>
-      </c>
-      <c r="M14" s="18">
-        <v>4690822.32</v>
-      </c>
-      <c r="N14" s="18">
-        <v>604.64200000000005</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="22">
-        <v>152</v>
-      </c>
-      <c r="F15" s="18">
-        <v>7512890.0329999998</v>
-      </c>
-      <c r="G15" s="18">
-        <v>4688200.6639999999</v>
-      </c>
-      <c r="H15" s="18">
-        <v>602.279</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="22">
-        <v>19</v>
-      </c>
-      <c r="L15" s="18">
-        <v>7513378.5779999997</v>
-      </c>
-      <c r="M15" s="18">
-        <v>4690849.2640000004</v>
-      </c>
-      <c r="N15" s="18">
-        <v>604.70899999999995</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="22">
-        <v>155</v>
-      </c>
-      <c r="F16" s="18">
-        <v>7512911.1310000001</v>
-      </c>
-      <c r="G16" s="18">
-        <v>4688155.2690000003</v>
-      </c>
-      <c r="H16" s="18">
-        <v>602.26599999999996</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K16" s="22">
-        <v>123</v>
-      </c>
-      <c r="L16" s="18">
-        <v>7513330.2640000004</v>
-      </c>
-      <c r="M16" s="18">
-        <v>4690842.0870000003</v>
-      </c>
-      <c r="N16" s="18">
-        <v>605.05399999999997</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E17" s="22">
-        <v>9</v>
-      </c>
-      <c r="F17" s="18">
-        <v>7512915.9336999999</v>
-      </c>
-      <c r="G17" s="18">
-        <v>4688194.9045000002</v>
-      </c>
-      <c r="H17" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" s="22">
-        <v>17</v>
-      </c>
-      <c r="L17" s="18">
-        <v>7513358.5389999999</v>
-      </c>
-      <c r="M17" s="18">
-        <v>4690822.3590000002</v>
-      </c>
-      <c r="N17" s="18">
-        <v>604.60199999999998</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E18" s="22">
-        <v>10</v>
-      </c>
-      <c r="F18" s="18">
-        <v>7512912.4574999996</v>
-      </c>
-      <c r="G18" s="18">
-        <v>4688193.57</v>
-      </c>
-      <c r="H18" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="22">
-        <v>20</v>
-      </c>
-      <c r="L18" s="18">
-        <v>7513386.9630000005</v>
-      </c>
-      <c r="M18" s="18">
-        <v>4690862.8320000004</v>
-      </c>
-      <c r="N18" s="18">
-        <v>604.92899999999997</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E19" s="22">
-        <v>11</v>
-      </c>
-      <c r="F19" s="18">
-        <v>7512912.7120000003</v>
-      </c>
-      <c r="G19" s="18">
-        <v>4688192.9069999997</v>
-      </c>
-      <c r="H19" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" s="22">
-        <v>69</v>
-      </c>
-      <c r="L19" s="18">
-        <v>7513337.3779999996</v>
-      </c>
-      <c r="M19" s="18">
-        <v>4690836.5530000003</v>
-      </c>
-      <c r="N19" s="18">
+      <c r="K25" s="18">
+        <v>132</v>
+      </c>
+      <c r="L25" s="14">
+        <v>7513329.3689999999</v>
+      </c>
+      <c r="M25" s="14">
+        <v>4690846.63</v>
+      </c>
+      <c r="N25" s="14">
         <v>607.98599999999999</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O25" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E20" s="22">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E26" s="18">
+        <v>58</v>
+      </c>
+      <c r="F26" s="14">
+        <v>7515269.4630000005</v>
+      </c>
+      <c r="G26" s="14">
+        <v>4688739.0549999997</v>
+      </c>
+      <c r="H26" s="14">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="18">
+        <v>133</v>
+      </c>
+      <c r="L26" s="14">
+        <v>7513338.0530000003</v>
+      </c>
+      <c r="M26" s="14">
+        <v>4690858.7259999998</v>
+      </c>
+      <c r="N26" s="14">
+        <v>607.98599999999999</v>
+      </c>
+      <c r="O26" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="18">
-        <v>7512908.3671000004</v>
-      </c>
-      <c r="G20" s="18">
-        <v>4688191.2390000001</v>
-      </c>
-      <c r="H20" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K20" s="22">
-        <v>70</v>
-      </c>
-      <c r="L20" s="18">
-        <v>7513343.1220000004</v>
-      </c>
-      <c r="M20" s="18">
-        <v>4690844.5829999996</v>
-      </c>
-      <c r="N20" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E21" s="22">
-        <v>15</v>
-      </c>
-      <c r="F21" s="18">
-        <v>7512905.0319999997</v>
-      </c>
-      <c r="G21" s="18">
-        <v>4688199.3990000002</v>
-      </c>
-      <c r="H21" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="22">
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E27" s="18">
+        <v>84</v>
+      </c>
+      <c r="F27" s="23">
+        <v>7515264.6198000005</v>
+      </c>
+      <c r="G27" s="23">
+        <v>4688744.0027999999</v>
+      </c>
+      <c r="H27" s="23">
+        <v>588.41700000000003</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E28" s="18">
+        <v>55</v>
+      </c>
+      <c r="F28" s="23">
+        <v>7515293.8770000003</v>
+      </c>
+      <c r="G28" s="23">
+        <v>4688742.0470000003</v>
+      </c>
+      <c r="H28" s="23">
+        <v>587.71400000000006</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E29" s="18">
+        <v>52</v>
+      </c>
+      <c r="F29" s="23">
+        <v>7515231.2230000002</v>
+      </c>
+      <c r="G29" s="23">
+        <v>4688740.2769999998</v>
+      </c>
+      <c r="H29" s="23">
+        <v>587.61199999999997</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E30" s="18">
+        <v>53</v>
+      </c>
+      <c r="F30" s="23">
+        <v>7515261.8739999998</v>
+      </c>
+      <c r="G30" s="23">
+        <v>4688757.7790000001</v>
+      </c>
+      <c r="H30" s="23">
+        <v>587.87800000000004</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="18">
         <v>71</v>
       </c>
-      <c r="L21" s="18">
-        <v>7513345.1220000004</v>
-      </c>
-      <c r="M21" s="18">
-        <v>4690843.176</v>
-      </c>
-      <c r="N21" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E22" s="22">
-        <v>167</v>
-      </c>
-      <c r="F22" s="18">
-        <v>7512912.8032999998</v>
-      </c>
-      <c r="G22" s="18">
-        <v>4688202.5635000002</v>
-      </c>
-      <c r="H22" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="22">
+      <c r="F31" s="23">
+        <v>7515251.9356000004</v>
+      </c>
+      <c r="G31" s="23">
+        <v>4688742.5897000004</v>
+      </c>
+      <c r="H31" s="23">
+        <v>593.86199999999997</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="18">
         <v>72</v>
       </c>
-      <c r="L22" s="18">
-        <v>7513350.1349999998</v>
-      </c>
-      <c r="M22" s="18">
-        <v>4690850.1849999996</v>
-      </c>
-      <c r="N22" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E23" s="22">
-        <v>7</v>
-      </c>
-      <c r="F23" s="18">
-        <v>7512916.9979999997</v>
-      </c>
-      <c r="G23" s="18">
-        <v>4688192.1320000002</v>
-      </c>
-      <c r="H23" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="22">
-        <v>130</v>
-      </c>
-      <c r="L23" s="18">
-        <v>7513331.6660000002</v>
-      </c>
-      <c r="M23" s="18">
-        <v>4690840.7719999999</v>
-      </c>
-      <c r="N23" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O23" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E24" s="22">
-        <v>12</v>
-      </c>
-      <c r="F24" s="18">
-        <v>7512911.5231999997</v>
-      </c>
-      <c r="G24" s="18">
-        <v>4688192.4506000001</v>
-      </c>
-      <c r="H24" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="22">
-        <v>131</v>
-      </c>
-      <c r="L24" s="18">
-        <v>7513333.6530999998</v>
-      </c>
-      <c r="M24" s="18">
-        <v>4690843.4441</v>
-      </c>
-      <c r="N24" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O24" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E25" s="22">
-        <v>13</v>
-      </c>
-      <c r="F25" s="18">
-        <v>7512912.3669999996</v>
-      </c>
-      <c r="G25" s="18">
-        <v>4688190.3370000003</v>
-      </c>
-      <c r="H25" s="18">
-        <v>601.94100000000003</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K25" s="22">
-        <v>132</v>
-      </c>
-      <c r="L25" s="18">
-        <v>7513329.3689999999</v>
-      </c>
-      <c r="M25" s="18">
-        <v>4690846.63</v>
-      </c>
-      <c r="N25" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O25" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E26" s="22">
-        <v>16</v>
-      </c>
-      <c r="F26" s="18">
-        <v>7512913.568</v>
-      </c>
-      <c r="G26" s="18">
-        <v>4688202.0793000003</v>
-      </c>
-      <c r="H26" s="18">
-        <v>601.69399999999996</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="22">
-        <v>133</v>
-      </c>
-      <c r="L26" s="18">
-        <v>7513338.0530000003</v>
-      </c>
-      <c r="M26" s="18">
-        <v>4690858.7259999998</v>
-      </c>
-      <c r="N26" s="18">
-        <v>607.98599999999999</v>
-      </c>
-      <c r="O26" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E27" s="22">
-        <v>309</v>
-      </c>
-      <c r="F27" s="27">
-        <v>7512950.6766999997</v>
-      </c>
-      <c r="G27" s="27">
-        <v>4688088.6792000001</v>
-      </c>
-      <c r="H27" s="27">
-        <v>601.86099999999999</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E28" s="22">
-        <v>19</v>
-      </c>
-      <c r="F28" s="27">
-        <v>7512904.5970000001</v>
-      </c>
-      <c r="G28" s="27">
-        <v>4688199.4639999997</v>
-      </c>
-      <c r="H28" s="27">
-        <v>607.77</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E29" s="22">
-        <v>20</v>
-      </c>
-      <c r="F29" s="27">
-        <v>7512908.5250000004</v>
-      </c>
-      <c r="G29" s="27">
-        <v>4688189.8779999996</v>
-      </c>
-      <c r="H29" s="27">
-        <v>607.77</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="5:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="28">
-        <v>21</v>
-      </c>
-      <c r="F30" s="29">
-        <v>7512916.9982000003</v>
-      </c>
-      <c r="G30" s="29">
-        <v>4688193.3232000005</v>
-      </c>
-      <c r="H30" s="29">
-        <v>607.77</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>14</v>
+      <c r="F32" s="23">
+        <v>7515262.1754000001</v>
+      </c>
+      <c r="G32" s="23">
+        <v>4688748.6966000004</v>
+      </c>
+      <c r="H32" s="23">
+        <v>593.86199999999997</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E33" s="18">
+        <v>73</v>
+      </c>
+      <c r="F33" s="23">
+        <v>7515267.4961000001</v>
+      </c>
+      <c r="G33" s="23">
+        <v>4688739.6835000003</v>
+      </c>
+      <c r="H33" s="23">
+        <v>593.86199999999997</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E34" s="18">
+        <v>86</v>
+      </c>
+      <c r="F34" s="23">
+        <v>7515257.2966</v>
+      </c>
+      <c r="G34" s="23">
+        <v>4688733.6007000003</v>
+      </c>
+      <c r="H34" s="23">
+        <v>593.86199999999997</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>